<commit_message>
Added stuff for blog post, plus playing with spirals
</commit_message>
<xml_diff>
--- a/Joes-CSS-Brown-Bag/moving-sun.xlsx
+++ b/Joes-CSS-Brown-Bag/moving-sun.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csudbery\Dropbox\IT Training\Web Stuff\Css Art\Joes-CSS-Brown-Bag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Dropbox\IT Training\Web Stuff\Css-Art\Joes-CSS-Brown-Bag\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Circle values" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="autoNoTable" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" calcMode="autoNoTable" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
@@ -192,6 +192,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -227,6 +244,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
@@ -430,11 +464,11 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <f>SQRT(100-(A2*A2))</f>
+        <f t="shared" ref="B2:B22" si="0">SQRT(100-(A2*A2))</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f>DEGREES(ATAN(B2/ABS(A2)))</f>
+        <f t="shared" ref="D2:D11" si="1">DEGREES(ATAN(B2/ABS(A2)))</f>
         <v>0</v>
       </c>
       <c r="E2">
@@ -449,11 +483,11 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <f>((A2*5)+50)*0.9</f>
+        <f t="shared" ref="I2:I22" si="2">((A2*5)+50)*0.9</f>
         <v>90</v>
       </c>
       <c r="J2" s="3">
-        <f>(B2*10)*0.9</f>
+        <f t="shared" ref="J2:J22" si="3">(B2*10)*0.9</f>
         <v>0</v>
       </c>
     </row>
@@ -462,11 +496,11 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <f>SQRT(100-(A3*A3))</f>
+        <f t="shared" si="0"/>
         <v>4.358898943540674</v>
       </c>
       <c r="D3">
-        <f>DEGREES(ATAN(B3/ABS(A3)))</f>
+        <f t="shared" si="1"/>
         <v>25.841932763167133</v>
       </c>
       <c r="E3">
@@ -477,15 +511,15 @@
         <v>5</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H22" si="0">(D3/180)*100</f>
+        <f t="shared" ref="H3:H22" si="4">(D3/180)*100</f>
         <v>14.356629312870631</v>
       </c>
       <c r="I3">
-        <f>((A3*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="J3" s="3">
-        <f>(B3*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>39.230090491866065</v>
       </c>
     </row>
@@ -494,11 +528,11 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <f>SQRT(100-(A4*A4))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D4">
-        <f>DEGREES(ATAN(B4/ABS(A4)))</f>
+        <f t="shared" si="1"/>
         <v>36.86989764584402</v>
       </c>
       <c r="E4">
@@ -509,15 +543,15 @@
         <v>10</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>20.483276469913346</v>
       </c>
       <c r="I4">
-        <f>((A4*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="J4" s="3">
-        <f>(B4*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
     </row>
@@ -526,11 +560,11 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <f>SQRT(100-(A5*A5))</f>
+        <f t="shared" si="0"/>
         <v>7.1414284285428504</v>
       </c>
       <c r="D5">
-        <f>DEGREES(ATAN(B5/ABS(A5)))</f>
+        <f t="shared" si="1"/>
         <v>45.572995999194298</v>
       </c>
       <c r="E5">
@@ -541,15 +575,15 @@
         <v>15</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>25.3183311106635</v>
       </c>
       <c r="I5">
-        <f>((A5*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>76.5</v>
       </c>
       <c r="J5" s="3">
-        <f>(B5*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>64.272855856885656</v>
       </c>
     </row>
@@ -558,11 +592,11 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f>SQRT(100-(A6*A6))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D6">
-        <f>DEGREES(ATAN(B6/ABS(A6)))</f>
+        <f t="shared" si="1"/>
         <v>53.13010235415598</v>
       </c>
       <c r="E6">
@@ -573,15 +607,15 @@
         <v>20</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>29.516723530086658</v>
       </c>
       <c r="I6">
-        <f>((A6*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="J6" s="3">
-        <f>(B6*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
     </row>
@@ -590,11 +624,11 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <f>SQRT(100-(A7*A7))</f>
+        <f t="shared" si="0"/>
         <v>8.6602540378443873</v>
       </c>
       <c r="D7">
-        <f>DEGREES(ATAN(B7/ABS(A7)))</f>
+        <f t="shared" si="1"/>
         <v>60.000000000000007</v>
       </c>
       <c r="E7">
@@ -605,15 +639,15 @@
         <v>25</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>33.333333333333336</v>
       </c>
       <c r="I7">
-        <f>((A7*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>67.5</v>
       </c>
       <c r="J7" s="3">
-        <f>(B7*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>77.942286340599495</v>
       </c>
     </row>
@@ -622,11 +656,11 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <f>SQRT(100-(A8*A8))</f>
+        <f t="shared" si="0"/>
         <v>9.1651513899116797</v>
       </c>
       <c r="D8">
-        <f>DEGREES(ATAN(B8/ABS(A8)))</f>
+        <f t="shared" si="1"/>
         <v>66.421821521798165</v>
       </c>
       <c r="E8">
@@ -637,15 +671,15 @@
         <v>30</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>36.901011956554534</v>
       </c>
       <c r="I8">
-        <f>((A8*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="J8" s="3">
-        <f>(B8*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>82.486362509205122</v>
       </c>
     </row>
@@ -654,11 +688,11 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <f>SQRT(100-(A9*A9))</f>
+        <f t="shared" si="0"/>
         <v>9.5393920141694561</v>
       </c>
       <c r="D9">
-        <f>DEGREES(ATAN(B9/ABS(A9)))</f>
+        <f t="shared" si="1"/>
         <v>72.542396876277905</v>
       </c>
       <c r="E9">
@@ -669,15 +703,15 @@
         <v>35</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>40.301331597932169</v>
       </c>
       <c r="I9">
-        <f>((A9*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>58.5</v>
       </c>
       <c r="J9" s="3">
-        <f>(B9*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>85.854528127525114</v>
       </c>
     </row>
@@ -686,11 +720,11 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <f>SQRT(100-(A10*A10))</f>
+        <f t="shared" si="0"/>
         <v>9.7979589711327115</v>
       </c>
       <c r="D10">
-        <f>DEGREES(ATAN(B10/ABS(A10)))</f>
+        <f t="shared" si="1"/>
         <v>78.463040967184526</v>
       </c>
       <c r="E10">
@@ -701,15 +735,15 @@
         <v>40</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>43.590578315102512</v>
       </c>
       <c r="I10">
-        <f>((A10*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="J10" s="3">
-        <f>(B10*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>88.181630740194407</v>
       </c>
     </row>
@@ -718,11 +752,11 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <f>SQRT(100-(A11*A11))</f>
+        <f t="shared" si="0"/>
         <v>9.9498743710661994</v>
       </c>
       <c r="D11">
-        <f>DEGREES(ATAN(B11/ABS(A11)))</f>
+        <f t="shared" si="1"/>
         <v>84.260829522733218</v>
       </c>
       <c r="E11">
@@ -733,15 +767,15 @@
         <v>45</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>46.811571957074008</v>
       </c>
       <c r="I11">
-        <f>((A11*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>49.5</v>
       </c>
       <c r="J11" s="3">
-        <f>(B11*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>89.548869339595797</v>
       </c>
     </row>
@@ -750,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <f>SQRT(100-(A12*A12))</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D12">
@@ -764,15 +798,15 @@
         <v>50</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="I12">
-        <f>((A12*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="J12" s="3">
-        <f>(B12*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
     </row>
@@ -781,7 +815,7 @@
         <v>-1</v>
       </c>
       <c r="B13">
-        <f>SQRT(100-(A13*A13))</f>
+        <f t="shared" si="0"/>
         <v>9.9498743710661994</v>
       </c>
       <c r="D13">
@@ -796,15 +830,15 @@
         <v>55</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>53.188428042925992</v>
       </c>
       <c r="I13">
-        <f>((A13*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>40.5</v>
       </c>
       <c r="J13" s="3">
-        <f>(B13*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>89.548869339595797</v>
       </c>
     </row>
@@ -813,7 +847,7 @@
         <v>-2</v>
       </c>
       <c r="B14">
-        <f>SQRT(100-(A14*A14))</f>
+        <f t="shared" si="0"/>
         <v>9.7979589711327115</v>
       </c>
       <c r="D14">
@@ -828,15 +862,15 @@
         <v>60</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>56.409421684897488</v>
       </c>
       <c r="I14">
-        <f>((A14*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="J14" s="3">
-        <f>(B14*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>88.181630740194407</v>
       </c>
     </row>
@@ -845,7 +879,7 @@
         <v>-3</v>
       </c>
       <c r="B15">
-        <f>SQRT(100-(A15*A15))</f>
+        <f t="shared" si="0"/>
         <v>9.5393920141694561</v>
       </c>
       <c r="D15">
@@ -860,15 +894,15 @@
         <v>65</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>59.698668402067831</v>
       </c>
       <c r="I15">
-        <f>((A15*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>31.5</v>
       </c>
       <c r="J15" s="3">
-        <f>(B15*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>85.854528127525114</v>
       </c>
     </row>
@@ -877,7 +911,7 @@
         <v>-4</v>
       </c>
       <c r="B16">
-        <f>SQRT(100-(A16*A16))</f>
+        <f t="shared" si="0"/>
         <v>9.1651513899116797</v>
       </c>
       <c r="D16">
@@ -892,15 +926,15 @@
         <v>70</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63.098988043445459</v>
       </c>
       <c r="I16">
-        <f>((A16*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="J16" s="3">
-        <f>(B16*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>82.486362509205122</v>
       </c>
     </row>
@@ -909,7 +943,7 @@
         <v>-5</v>
       </c>
       <c r="B17">
-        <f>SQRT(100-(A17*A17))</f>
+        <f t="shared" si="0"/>
         <v>8.6602540378443873</v>
       </c>
       <c r="D17">
@@ -924,15 +958,15 @@
         <v>75</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>66.666666666666657</v>
       </c>
       <c r="I17">
-        <f>((A17*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>22.5</v>
       </c>
       <c r="J17" s="3">
-        <f>(B17*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>77.942286340599495</v>
       </c>
     </row>
@@ -941,7 +975,7 @@
         <v>-6</v>
       </c>
       <c r="B18">
-        <f>SQRT(100-(A18*A18))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D18">
@@ -956,15 +990,15 @@
         <v>80</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70.483276469913349</v>
       </c>
       <c r="I18">
-        <f>((A18*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="J18" s="3">
-        <f>(B18*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
     </row>
@@ -973,7 +1007,7 @@
         <v>-7</v>
       </c>
       <c r="B19">
-        <f>SQRT(100-(A19*A19))</f>
+        <f t="shared" si="0"/>
         <v>7.1414284285428504</v>
       </c>
       <c r="D19">
@@ -988,15 +1022,15 @@
         <v>85</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>74.681668889336507</v>
       </c>
       <c r="I19">
-        <f>((A19*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>13.5</v>
       </c>
       <c r="J19" s="3">
-        <f>(B19*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>64.272855856885656</v>
       </c>
     </row>
@@ -1005,7 +1039,7 @@
         <v>-8</v>
       </c>
       <c r="B20">
-        <f>SQRT(100-(A20*A20))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D20">
@@ -1020,15 +1054,15 @@
         <v>90</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>79.516723530086651</v>
       </c>
       <c r="I20">
-        <f>((A20*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J20" s="3">
-        <f>(B20*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
     </row>
@@ -1037,7 +1071,7 @@
         <v>-9</v>
       </c>
       <c r="B21">
-        <f>SQRT(100-(A21*A21))</f>
+        <f t="shared" si="0"/>
         <v>4.358898943540674</v>
       </c>
       <c r="D21">
@@ -1052,15 +1086,15 @@
         <v>95</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>85.643370687129377</v>
       </c>
       <c r="I21">
-        <f>((A21*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
       <c r="J21" s="3">
-        <f>(B21*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>39.230090491866065</v>
       </c>
     </row>
@@ -1069,7 +1103,7 @@
         <v>-10</v>
       </c>
       <c r="B22">
-        <f>SQRT(100-(A22*A22))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D22">
@@ -1084,15 +1118,15 @@
         <v>100</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="I22">
-        <f>((A22*5)+50)*0.9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <f>(B22*10)*0.9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made some tidy-up changes ready for brown bag
</commit_message>
<xml_diff>
--- a/Joes-CSS-Brown-Bag/moving-sun.xlsx
+++ b/Joes-CSS-Brown-Bag/moving-sun.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Dropbox\IT Training\Web Stuff\Css-Art\Joes-CSS-Brown-Bag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csudbery\Dropbox\IT Training\Web Stuff\Css-Art\Joes-CSS-Brown-Bag\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Circle values" sheetId="1" r:id="rId1"/>
+    <sheet name="Circle values (no timing)" sheetId="2" r:id="rId1"/>
+    <sheet name="Circle values" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" calcMode="autoNoTable" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="152511" calcMode="autoNoTable" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
@@ -192,23 +193,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -244,23 +228,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,11 +380,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B22" si="0">SQRT(100-(A2*A2))</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D22" si="1">((A2*5)+50)*0.9</f>
+        <v>90</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:E22" si="2">(B2*10)*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>4.358898943540674</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>85.5</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="2"/>
+        <v>39.230090491866065</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>7.1414284285428504</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>76.5</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="2"/>
+        <v>64.272855856885656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>8.6602540378443873</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>67.5</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="2"/>
+        <v>77.942286340599495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>9.1651513899116797</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="2"/>
+        <v>82.486362509205122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>9.5393920141694561</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>58.5</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="2"/>
+        <v>85.854528127525114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>9.7979589711327115</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="2"/>
+        <v>88.181630740194407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>9.9498743710661994</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>49.5</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="2"/>
+        <v>89.548869339595797</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>9.9498743710661994</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>40.5</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="2"/>
+        <v>89.548869339595797</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-2</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>9.7979589711327115</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>88.181630740194407</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-3</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>9.5393920141694561</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>31.5</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="2"/>
+        <v>85.854528127525114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-4</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>9.1651513899116797</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="2"/>
+        <v>82.486362509205122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-5</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>8.6602540378443873</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>22.5</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="2"/>
+        <v>77.942286340599495</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-6</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-7</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>7.1414284285428504</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>13.5</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="2"/>
+        <v>64.272855856885656</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-8</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-9</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>4.358898943540674</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="2"/>
+        <v>39.230090491866065</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-10</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>